<commit_message>
update ISBN in links
</commit_message>
<xml_diff>
--- a/books/md/_content.xlsx
+++ b/books/md/_content.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>shortName</t>
   </si>
@@ -79,16 +79,36 @@
   </si>
   <si>
     <t>Max Tegmark</t>
+  </si>
+  <si>
+    <t>0451166892</t>
+  </si>
+  <si>
+    <t>0812983416</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Menlo Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Menlo Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="11"/>
       <name val="Menlo Regular"/>
       <family val="2"/>
     </font>
@@ -110,13 +130,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,11 +471,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
@@ -487,7 +510,7 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1101946598</v>
       </c>
       <c r="E2">
@@ -507,8 +530,8 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
-        <v>812983416</v>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E3">
         <v>2015</v>
@@ -527,8 +550,8 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>451166892</v>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E4">
         <v>1989</v>
@@ -547,7 +570,7 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1585166448</v>
       </c>
       <c r="E5" t="s">
@@ -556,6 +579,489 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="4:4">
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="4:4">
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="4:4">
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="4:4">
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="4:4">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="4:4">
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="4:4">
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="4:4">
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="4:4">
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="4:4">
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="4:4">
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="4:4">
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="4:4">
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="4:4">
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="4:4">
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="4:4">
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="4:4">
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="4:4">
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="4:4">
+      <c r="D63" s="1"/>
+    </row>
+    <row r="64" spans="4:4">
+      <c r="D64" s="1"/>
+    </row>
+    <row r="65" spans="4:4">
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="4:4">
+      <c r="D66" s="1"/>
+    </row>
+    <row r="67" spans="4:4">
+      <c r="D67" s="1"/>
+    </row>
+    <row r="68" spans="4:4">
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69" spans="4:4">
+      <c r="D69" s="1"/>
+    </row>
+    <row r="70" spans="4:4">
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="4:4">
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="4:4">
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73" spans="4:4">
+      <c r="D73" s="1"/>
+    </row>
+    <row r="74" spans="4:4">
+      <c r="D74" s="1"/>
+    </row>
+    <row r="75" spans="4:4">
+      <c r="D75" s="1"/>
+    </row>
+    <row r="76" spans="4:4">
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77" spans="4:4">
+      <c r="D77" s="1"/>
+    </row>
+    <row r="78" spans="4:4">
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="4:4">
+      <c r="D79" s="1"/>
+    </row>
+    <row r="80" spans="4:4">
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="4:4">
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="4:4">
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="4:4">
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="4:4">
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="4:4">
+      <c r="D85" s="1"/>
+    </row>
+    <row r="86" spans="4:4">
+      <c r="D86" s="1"/>
+    </row>
+    <row r="87" spans="4:4">
+      <c r="D87" s="1"/>
+    </row>
+    <row r="88" spans="4:4">
+      <c r="D88" s="1"/>
+    </row>
+    <row r="89" spans="4:4">
+      <c r="D89" s="1"/>
+    </row>
+    <row r="90" spans="4:4">
+      <c r="D90" s="1"/>
+    </row>
+    <row r="91" spans="4:4">
+      <c r="D91" s="1"/>
+    </row>
+    <row r="92" spans="4:4">
+      <c r="D92" s="1"/>
+    </row>
+    <row r="93" spans="4:4">
+      <c r="D93" s="1"/>
+    </row>
+    <row r="94" spans="4:4">
+      <c r="D94" s="1"/>
+    </row>
+    <row r="95" spans="4:4">
+      <c r="D95" s="1"/>
+    </row>
+    <row r="96" spans="4:4">
+      <c r="D96" s="1"/>
+    </row>
+    <row r="97" spans="4:4">
+      <c r="D97" s="1"/>
+    </row>
+    <row r="98" spans="4:4">
+      <c r="D98" s="1"/>
+    </row>
+    <row r="99" spans="4:4">
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="4:4">
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="4:4">
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="4:4">
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="4:4">
+      <c r="D103" s="1"/>
+    </row>
+    <row r="104" spans="4:4">
+      <c r="D104" s="1"/>
+    </row>
+    <row r="105" spans="4:4">
+      <c r="D105" s="1"/>
+    </row>
+    <row r="106" spans="4:4">
+      <c r="D106" s="1"/>
+    </row>
+    <row r="107" spans="4:4">
+      <c r="D107" s="1"/>
+    </row>
+    <row r="108" spans="4:4">
+      <c r="D108" s="1"/>
+    </row>
+    <row r="109" spans="4:4">
+      <c r="D109" s="1"/>
+    </row>
+    <row r="110" spans="4:4">
+      <c r="D110" s="1"/>
+    </row>
+    <row r="111" spans="4:4">
+      <c r="D111" s="1"/>
+    </row>
+    <row r="112" spans="4:4">
+      <c r="D112" s="1"/>
+    </row>
+    <row r="113" spans="4:4">
+      <c r="D113" s="1"/>
+    </row>
+    <row r="114" spans="4:4">
+      <c r="D114" s="1"/>
+    </row>
+    <row r="115" spans="4:4">
+      <c r="D115" s="1"/>
+    </row>
+    <row r="116" spans="4:4">
+      <c r="D116" s="1"/>
+    </row>
+    <row r="117" spans="4:4">
+      <c r="D117" s="1"/>
+    </row>
+    <row r="118" spans="4:4">
+      <c r="D118" s="1"/>
+    </row>
+    <row r="119" spans="4:4">
+      <c r="D119" s="1"/>
+    </row>
+    <row r="120" spans="4:4">
+      <c r="D120" s="1"/>
+    </row>
+    <row r="121" spans="4:4">
+      <c r="D121" s="1"/>
+    </row>
+    <row r="122" spans="4:4">
+      <c r="D122" s="1"/>
+    </row>
+    <row r="123" spans="4:4">
+      <c r="D123" s="1"/>
+    </row>
+    <row r="124" spans="4:4">
+      <c r="D124" s="1"/>
+    </row>
+    <row r="125" spans="4:4">
+      <c r="D125" s="1"/>
+    </row>
+    <row r="126" spans="4:4">
+      <c r="D126" s="1"/>
+    </row>
+    <row r="127" spans="4:4">
+      <c r="D127" s="1"/>
+    </row>
+    <row r="128" spans="4:4">
+      <c r="D128" s="1"/>
+    </row>
+    <row r="129" spans="4:4">
+      <c r="D129" s="1"/>
+    </row>
+    <row r="130" spans="4:4">
+      <c r="D130" s="1"/>
+    </row>
+    <row r="131" spans="4:4">
+      <c r="D131" s="1"/>
+    </row>
+    <row r="132" spans="4:4">
+      <c r="D132" s="1"/>
+    </row>
+    <row r="133" spans="4:4">
+      <c r="D133" s="1"/>
+    </row>
+    <row r="134" spans="4:4">
+      <c r="D134" s="1"/>
+    </row>
+    <row r="135" spans="4:4">
+      <c r="D135" s="1"/>
+    </row>
+    <row r="136" spans="4:4">
+      <c r="D136" s="1"/>
+    </row>
+    <row r="137" spans="4:4">
+      <c r="D137" s="1"/>
+    </row>
+    <row r="138" spans="4:4">
+      <c r="D138" s="1"/>
+    </row>
+    <row r="139" spans="4:4">
+      <c r="D139" s="1"/>
+    </row>
+    <row r="140" spans="4:4">
+      <c r="D140" s="1"/>
+    </row>
+    <row r="141" spans="4:4">
+      <c r="D141" s="1"/>
+    </row>
+    <row r="142" spans="4:4">
+      <c r="D142" s="1"/>
+    </row>
+    <row r="143" spans="4:4">
+      <c r="D143" s="1"/>
+    </row>
+    <row r="144" spans="4:4">
+      <c r="D144" s="1"/>
+    </row>
+    <row r="145" spans="4:4">
+      <c r="D145" s="1"/>
+    </row>
+    <row r="146" spans="4:4">
+      <c r="D146" s="1"/>
+    </row>
+    <row r="147" spans="4:4">
+      <c r="D147" s="1"/>
+    </row>
+    <row r="148" spans="4:4">
+      <c r="D148" s="1"/>
+    </row>
+    <row r="149" spans="4:4">
+      <c r="D149" s="1"/>
+    </row>
+    <row r="150" spans="4:4">
+      <c r="D150" s="1"/>
+    </row>
+    <row r="151" spans="4:4">
+      <c r="D151" s="1"/>
+    </row>
+    <row r="152" spans="4:4">
+      <c r="D152" s="1"/>
+    </row>
+    <row r="153" spans="4:4">
+      <c r="D153" s="1"/>
+    </row>
+    <row r="154" spans="4:4">
+      <c r="D154" s="1"/>
+    </row>
+    <row r="155" spans="4:4">
+      <c r="D155" s="1"/>
+    </row>
+    <row r="156" spans="4:4">
+      <c r="D156" s="1"/>
+    </row>
+    <row r="157" spans="4:4">
+      <c r="D157" s="1"/>
+    </row>
+    <row r="158" spans="4:4">
+      <c r="D158" s="1"/>
+    </row>
+    <row r="159" spans="4:4">
+      <c r="D159" s="1"/>
+    </row>
+    <row r="160" spans="4:4">
+      <c r="D160" s="1"/>
+    </row>
+    <row r="161" spans="4:4">
+      <c r="D161" s="1"/>
+    </row>
+    <row r="162" spans="4:4">
+      <c r="D162" s="1"/>
+    </row>
+    <row r="163" spans="4:4">
+      <c r="D163" s="1"/>
+    </row>
+    <row r="164" spans="4:4">
+      <c r="D164" s="1"/>
+    </row>
+    <row r="165" spans="4:4">
+      <c r="D165" s="1"/>
+    </row>
+    <row r="166" spans="4:4">
+      <c r="D166" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update Life 3.0 notes
</commit_message>
<xml_diff>
--- a/books/md/_content.xlsx
+++ b/books/md/_content.xlsx
@@ -473,7 +473,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>